<commit_message>
Updated explaination and vms code
</commit_message>
<xml_diff>
--- a/output/BSI_Processed_Report.xlsx
+++ b/output/BSI_Processed_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agentic AI\Projects\vms\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7DE9F6-D592-4EAB-B9C7-051970987B90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962BD8D1-7742-4C2D-BB4D-EBC42572CF31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Data" sheetId="1" r:id="rId1"/>
@@ -53999,7 +53999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -61879,8 +61879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>